<commit_message>
ElectionResults & some changes
</commit_message>
<xml_diff>
--- a/candidates/Kandidierendenlisten.xlsx
+++ b/candidates/Kandidierendenlisten.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gian\Documents\NetBeansProjects\VoteGen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="330" windowWidth="22755" windowHeight="9750"/>
+    <workbookView xWindow="720" yWindow="330" windowWidth="22755" windowHeight="9750" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="26">
   <si>
     <t>Kandidierendenliste</t>
   </si>
@@ -81,9 +76,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>HSR2013</t>
-  </si>
-  <si>
     <t>Cadosch</t>
   </si>
   <si>
@@ -100,6 +92,21 @@
   </si>
   <si>
     <t>Giovanni</t>
+  </si>
+  <si>
+    <t>Lehrer</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Poltera</t>
+  </si>
+  <si>
+    <t>Gian</t>
+  </si>
+  <si>
+    <t>Informatiker</t>
   </si>
 </sst>
 </file>
@@ -274,9 +281,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -314,9 +321,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -351,7 +358,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -386,7 +393,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -562,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +611,7 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -659,10 +666,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -676,10 +683,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -693,10 +700,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -3430,8 +3437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3462,14 +3469,18 @@
         <v>1</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
+      <c r="C4" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
@@ -3522,8 +3533,12 @@
       <c r="A9" s="6">
         <v>1</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="6"/>

</xml_diff>